<commit_message>
updated timing for nilpotent_monoid2
</commit_message>
<xml_diff>
--- a/docs/nilpotent_monoid2.xlsx
+++ b/docs/nilpotent_monoid2.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nilpotent_2_1 run times" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Bands" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t xml:space="preserve">Run on</t>
   </si>
@@ -137,6 +138,48 @@
   </si>
   <si>
     <t xml:space="preserve">x1x2x3x4x5x6 = y1y2y3y4y5y6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N^1_2: x^2=x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1, page 5 https://arxiv.org/pdf/1911.05817.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to find first model in minimum order (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total time starting from order 2 to minimum order (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subvarieties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varieties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4=H4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4rG4 = I4rH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4rG4 = I4rI4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4rG4 = H4rI4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G4r = H4r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no models found up to order 8, 97791.43 sec</t>
   </si>
 </sst>
 </file>
@@ -152,6 +195,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,6 +274,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -251,11 +299,11 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.48"/>
@@ -637,4 +685,669 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:H45"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.15"/>
+  </cols>
+  <sheetData>
+    <row r="2" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>240.13</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>389.42</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>83.76</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>245.3</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>16.26</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>23.56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>6180.96</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>9504.92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>2044</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>5857.61</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>19.98</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>26.29</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>31145</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>66091.73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>106433.51</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>254139.62</v>
+      </c>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>80338</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>218693.81</v>
+      </c>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>56313.06</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>104307.58</v>
+      </c>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>845.4</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>4902.48</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>2558.36</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>5639.7</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>10361.2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="G45" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>